<commit_message>
Modified absence/presence to include temperature all in one. Make absence-presence plot here now. Version for survey temps and continuous water temps.
</commit_message>
<xml_diff>
--- a/SpeciesTables/SpeciesTable_Veg_Clams.xlsx
+++ b/SpeciesTables/SpeciesTable_Veg_Clams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/catarina_pien_water_ca_gov/Documents/Work/ClimateChange/R_code/TempSynthesis/SpeciesTables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{6D7205FA-9361-450C-9E83-A003128A1E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{610756E4-F20B-4382-A165-2DDE02B6D4E8}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{6D7205FA-9361-450C-9E83-A003128A1E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82056D1D-4EEE-4026-8ACD-6D7FFBD33016}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CFB1209-DCFA-45F1-8D34-2EFE0A1507EC}"/>
+    <workbookView xWindow="-23355" yWindow="345" windowWidth="21600" windowHeight="11265" xr2:uid="{1CFB1209-DCFA-45F1-8D34-2EFE0A1507EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="20">
   <si>
     <t>Region</t>
   </si>
@@ -48,24 +48,9 @@
     <t>Winter</t>
   </si>
   <si>
-    <t>Egeria</t>
-  </si>
-  <si>
     <t>Spring</t>
   </si>
   <si>
-    <t>Arundo</t>
-  </si>
-  <si>
-    <t>Hyacinth</t>
-  </si>
-  <si>
-    <t>South Delta</t>
-  </si>
-  <si>
-    <t>Central Delta</t>
-  </si>
-  <si>
     <t>Suisun Bay</t>
   </si>
   <si>
@@ -81,16 +66,34 @@
     <t>Microcystis</t>
   </si>
   <si>
-    <t>Potamocorbula</t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
     <t>Fall</t>
   </si>
   <si>
-    <t>Corbicula</t>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>Brazilian Waterweed</t>
+  </si>
+  <si>
+    <t>Overbite Clam</t>
+  </si>
+  <si>
+    <t>Asian Clam</t>
+  </si>
+  <si>
+    <t>Giant Reed EAV</t>
+  </si>
+  <si>
+    <t>Water Hyacinth FAV</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>LifeStage</t>
   </si>
 </sst>
 </file>
@@ -481,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A30CCF-156B-4905-9E5E-A387ACE5A25E}">
   <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,9 +499,11 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -508,11 +513,11 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -520,10 +525,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -531,10 +536,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -542,7 +547,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -550,43 +555,43 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
@@ -594,43 +599,43 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
         <v>3</v>
@@ -638,43 +643,43 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
         <v>3</v>
@@ -682,43 +687,43 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
         <v>3</v>
@@ -726,43 +731,43 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
         <v>3</v>
@@ -773,10 +778,10 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -784,10 +789,10 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -795,10 +800,10 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -806,7 +811,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D29" t="s">
         <v>3</v>
@@ -814,44 +819,44 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
         <v>3</v>
@@ -859,43 +864,43 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D37" t="s">
         <v>3</v>
@@ -903,43 +908,43 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D41" t="s">
         <v>3</v>
@@ -947,43 +952,43 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D45" t="s">
         <v>3</v>
@@ -991,43 +996,43 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D49" t="s">
         <v>3</v>
@@ -1038,11 +1043,11 @@
         <v>2</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1050,11 +1055,11 @@
         <v>2</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1062,11 +1067,11 @@
         <v>2</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1074,7 +1079,7 @@
         <v>2</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D53" t="s">
         <v>3</v>
@@ -1082,45 +1087,45 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D57" t="s">
         <v>3</v>
@@ -1128,45 +1133,45 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D61" t="s">
         <v>3</v>
@@ -1174,43 +1179,43 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D64" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D65" t="s">
         <v>3</v>
@@ -1218,43 +1223,43 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B66" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D67" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D68" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D69" t="s">
         <v>3</v>
@@ -1262,43 +1267,43 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D71" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D72" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D73" t="s">
         <v>3</v>
@@ -1309,11 +1314,11 @@
         <v>2</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1321,166 +1326,166 @@
         <v>2</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B80" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D80" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B81" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D81" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B82" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D82" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B83" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D83" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B84" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D84" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B85" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D85" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B86" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D86" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D87" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B88" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D88" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B89" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D89" t="s">
         <v>3</v>
@@ -1488,43 +1493,43 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B90" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D90" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B91" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D91" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B92" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D92" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B93" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D93" t="s">
         <v>3</v>
@@ -1532,43 +1537,43 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B94" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B95" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D95" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B96" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D96" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B97" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D97" t="s">
         <v>3</v>
@@ -1579,10 +1584,10 @@
         <v>2</v>
       </c>
       <c r="B98" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D98" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1590,10 +1595,10 @@
         <v>2</v>
       </c>
       <c r="B99" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D99" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1601,10 +1606,10 @@
         <v>2</v>
       </c>
       <c r="B100" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D100" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1612,7 +1617,7 @@
         <v>2</v>
       </c>
       <c r="B101" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D101" t="s">
         <v>3</v>
@@ -1620,44 +1625,44 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C102" s="3"/>
       <c r="D102" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B103" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D103" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B104" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D104" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B105" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D105" t="s">
         <v>3</v>
@@ -1665,43 +1670,43 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B106" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D106" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B107" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D107" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B108" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D108" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B109" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D109" t="s">
         <v>3</v>
@@ -1709,43 +1714,43 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B110" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D110" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B111" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D111" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B112" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D112" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B113" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D113" t="s">
         <v>3</v>
@@ -1753,43 +1758,43 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B114" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D114" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B115" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D115" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B116" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D116" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D117" t="s">
         <v>3</v>
@@ -1797,43 +1802,43 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B118" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D118" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B119" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D119" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B120" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D120" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B121" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D121" t="s">
         <v>3</v>

</xml_diff>